<commit_message>
up-to-date db, processed players info with new status, excel file of players table, removed duplicate elements / bootstrap-static file
</commit_message>
<xml_diff>
--- a/players.xlsx
+++ b/players.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -630,7 +630,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -880,7 +880,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -952,7 +952,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1520,7 +1520,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -3720,7 +3720,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
@@ -3924,7 +3924,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F101" t="inlineStr"/>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F104" t="inlineStr"/>
@@ -4196,7 +4196,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -4514,7 +4514,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -4552,7 +4552,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>n</t>
         </is>
       </c>
       <c r="F119" t="inlineStr"/>
@@ -4586,7 +4586,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -4862,7 +4862,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F128" t="inlineStr"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -5040,7 +5040,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -5112,7 +5112,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F138" t="inlineStr"/>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -5430,7 +5430,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -5536,7 +5536,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F147" t="inlineStr"/>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F148" t="inlineStr"/>
@@ -5604,7 +5604,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -5642,7 +5642,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F150" t="inlineStr"/>
@@ -5812,7 +5812,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F172" t="inlineStr"/>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F175" t="inlineStr"/>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F176" t="inlineStr"/>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F180" t="inlineStr"/>
@@ -6870,7 +6870,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F186" t="inlineStr"/>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6976,7 +6976,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F189" t="inlineStr"/>
@@ -7010,7 +7010,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F190" t="inlineStr"/>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F191" t="inlineStr"/>
@@ -7078,7 +7078,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F192" t="inlineStr"/>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F193" t="inlineStr"/>
@@ -7146,7 +7146,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F194" t="inlineStr"/>
@@ -7214,7 +7214,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -7286,7 +7286,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -7392,7 +7392,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F201" t="inlineStr"/>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F202" t="inlineStr"/>
@@ -7596,7 +7596,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -7668,7 +7668,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F209" t="inlineStr"/>
@@ -7702,7 +7702,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -7740,7 +7740,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -7816,7 +7816,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7854,7 +7854,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F214" t="inlineStr"/>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7994,7 +7994,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -8202,7 +8202,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F224" t="inlineStr"/>
@@ -8304,7 +8304,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -8410,7 +8410,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F230" t="inlineStr"/>
@@ -8580,7 +8580,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F235" t="inlineStr"/>
@@ -8648,7 +8648,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F237" t="inlineStr"/>
@@ -8682,7 +8682,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F238" t="inlineStr"/>
@@ -8988,7 +8988,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -9026,7 +9026,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F248" t="inlineStr"/>
@@ -9060,7 +9060,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F249" t="inlineStr"/>
@@ -9434,7 +9434,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F260" t="inlineStr"/>
@@ -9570,7 +9570,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -9608,7 +9608,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F265" t="inlineStr"/>
@@ -9642,7 +9642,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -9748,7 +9748,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F269" t="inlineStr"/>
@@ -9986,7 +9986,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -10092,7 +10092,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -10164,7 +10164,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F281" t="inlineStr"/>
@@ -10198,7 +10198,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -10508,7 +10508,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -10546,7 +10546,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -10618,7 +10618,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -10656,7 +10656,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -10728,7 +10728,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F297" t="inlineStr"/>
@@ -10762,7 +10762,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -10800,7 +10800,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -10838,7 +10838,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F300" t="inlineStr"/>
@@ -10940,7 +10940,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -10978,7 +10978,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -11016,7 +11016,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -11122,7 +11122,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -11160,7 +11160,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -11304,7 +11304,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F313" t="inlineStr"/>
@@ -11338,7 +11338,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -11512,7 +11512,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F319" t="inlineStr"/>
@@ -11580,7 +11580,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F321" t="inlineStr"/>
@@ -11750,7 +11750,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F326" t="inlineStr"/>
@@ -11886,7 +11886,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F330" t="inlineStr"/>
@@ -11920,7 +11920,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F331" t="inlineStr"/>
@@ -12022,7 +12022,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F334" t="inlineStr"/>
@@ -12158,7 +12158,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>n</t>
         </is>
       </c>
       <c r="F338" t="inlineStr"/>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F339" t="inlineStr"/>
@@ -12294,7 +12294,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -12332,7 +12332,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -12370,7 +12370,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -12408,7 +12408,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -12548,7 +12548,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F349" t="inlineStr"/>
@@ -12582,7 +12582,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -12620,7 +12620,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -12692,7 +12692,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -12730,7 +12730,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -12768,7 +12768,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -12806,7 +12806,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -12946,7 +12946,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F360" t="inlineStr"/>
@@ -13150,7 +13150,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -13256,7 +13256,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -13294,7 +13294,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -13332,7 +13332,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F371" t="inlineStr"/>
@@ -13366,7 +13366,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F372" t="inlineStr"/>
@@ -13400,7 +13400,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -13438,7 +13438,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -13578,7 +13578,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -13956,7 +13956,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F389" t="inlineStr"/>
@@ -13990,7 +13990,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F390" t="inlineStr"/>
@@ -14024,7 +14024,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F391" t="inlineStr"/>
@@ -14058,7 +14058,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -14198,7 +14198,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -14236,7 +14236,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -14308,7 +14308,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -14448,7 +14448,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -14520,7 +14520,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F405" t="inlineStr"/>
@@ -14554,7 +14554,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -14592,7 +14592,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -14630,7 +14630,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -14668,7 +14668,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F409" t="inlineStr"/>
@@ -14906,7 +14906,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -14944,7 +14944,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -14982,7 +14982,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F418" t="inlineStr"/>
@@ -15084,7 +15084,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F421" t="inlineStr"/>
@@ -15152,7 +15152,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F423" t="inlineStr"/>
@@ -15220,7 +15220,7 @@
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -15292,7 +15292,7 @@
       </c>
       <c r="E427" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F427" t="inlineStr"/>
@@ -15326,7 +15326,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -15432,7 +15432,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -15470,7 +15470,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F432" t="inlineStr"/>
@@ -15504,7 +15504,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F433" t="inlineStr"/>
@@ -15538,7 +15538,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
@@ -15678,7 +15678,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -15784,7 +15784,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F441" t="inlineStr"/>
@@ -15954,7 +15954,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F446" t="inlineStr"/>
@@ -16022,7 +16022,7 @@
       </c>
       <c r="E448" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -16060,7 +16060,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F449" t="inlineStr"/>
@@ -16196,7 +16196,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F453" t="inlineStr"/>
@@ -16366,7 +16366,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F458" t="inlineStr"/>
@@ -16434,7 +16434,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F460" t="inlineStr"/>
@@ -16604,7 +16604,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F465" t="inlineStr"/>
@@ -17012,7 +17012,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F477" t="inlineStr"/>
@@ -17046,7 +17046,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F478" t="inlineStr"/>
@@ -17080,7 +17080,7 @@
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F479" t="inlineStr"/>
@@ -17182,7 +17182,7 @@
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F482" t="inlineStr"/>
@@ -17250,7 +17250,7 @@
       </c>
       <c r="E484" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F484" t="inlineStr"/>
@@ -17318,7 +17318,7 @@
       </c>
       <c r="E486" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F486" t="inlineStr"/>
@@ -17352,7 +17352,7 @@
       </c>
       <c r="E487" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F487" t="inlineStr"/>
@@ -17386,7 +17386,7 @@
       </c>
       <c r="E488" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F488" t="inlineStr"/>
@@ -17420,7 +17420,7 @@
       </c>
       <c r="E489" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F489" t="inlineStr"/>
@@ -17556,7 +17556,7 @@
       </c>
       <c r="E493" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F493" t="inlineStr"/>
@@ -17624,7 +17624,7 @@
       </c>
       <c r="E495" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F495" t="inlineStr"/>
@@ -17726,7 +17726,7 @@
       </c>
       <c r="E498" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F498" t="inlineStr">
@@ -17798,7 +17798,7 @@
       </c>
       <c r="E500" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F500" t="inlineStr">
@@ -17836,7 +17836,7 @@
       </c>
       <c r="E501" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F501" t="inlineStr">
@@ -17874,7 +17874,7 @@
       </c>
       <c r="E502" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F502" t="inlineStr">
@@ -17912,7 +17912,7 @@
       </c>
       <c r="E503" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F503" t="inlineStr">
@@ -17984,7 +17984,7 @@
       </c>
       <c r="E505" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F505" t="inlineStr">
@@ -18056,7 +18056,7 @@
       </c>
       <c r="E507" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F507" t="inlineStr">
@@ -18094,7 +18094,7 @@
       </c>
       <c r="E508" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F508" t="inlineStr">
@@ -18166,7 +18166,7 @@
       </c>
       <c r="E510" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F510" t="inlineStr">
@@ -18238,7 +18238,7 @@
       </c>
       <c r="E512" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F512" t="inlineStr">
@@ -18344,7 +18344,7 @@
       </c>
       <c r="E515" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F515" t="inlineStr"/>
@@ -18412,7 +18412,7 @@
       </c>
       <c r="E517" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F517" t="inlineStr">
@@ -18518,7 +18518,7 @@
       </c>
       <c r="E520" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F520" t="inlineStr">
@@ -18556,7 +18556,7 @@
       </c>
       <c r="E521" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F521" t="inlineStr">
@@ -18662,7 +18662,7 @@
       </c>
       <c r="E524" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F524" t="inlineStr">
@@ -18768,7 +18768,7 @@
       </c>
       <c r="E527" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F527" t="inlineStr">
@@ -19010,7 +19010,7 @@
       </c>
       <c r="E534" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F534" t="inlineStr">
@@ -19082,7 +19082,7 @@
       </c>
       <c r="E536" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F536" t="inlineStr">
@@ -19222,7 +19222,7 @@
       </c>
       <c r="E540" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F540" t="inlineStr">
@@ -19260,7 +19260,7 @@
       </c>
       <c r="E541" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F541" t="inlineStr">
@@ -19298,7 +19298,7 @@
       </c>
       <c r="E542" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F542" t="inlineStr">
@@ -19404,7 +19404,7 @@
       </c>
       <c r="E545" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F545" t="inlineStr">
@@ -19578,7 +19578,7 @@
       </c>
       <c r="E550" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F550" t="inlineStr"/>
@@ -19816,7 +19816,7 @@
       </c>
       <c r="E557" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F557" t="inlineStr"/>
@@ -19884,7 +19884,7 @@
       </c>
       <c r="E559" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F559" t="inlineStr">
@@ -20092,7 +20092,7 @@
       </c>
       <c r="E565" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F565" t="inlineStr">
@@ -20266,7 +20266,7 @@
       </c>
       <c r="E570" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F570" t="inlineStr">
@@ -20338,7 +20338,7 @@
       </c>
       <c r="E572" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>u</t>
         </is>
       </c>
       <c r="F572" t="inlineStr"/>
@@ -20474,7 +20474,7 @@
       </c>
       <c r="E576" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F576" t="inlineStr"/>
@@ -20814,7 +20814,7 @@
       </c>
       <c r="E586" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F586" t="inlineStr">
@@ -21226,7 +21226,7 @@
       </c>
       <c r="E598" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F598" t="inlineStr">
@@ -21298,7 +21298,7 @@
       </c>
       <c r="E600" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F600" t="inlineStr">
@@ -21370,7 +21370,7 @@
       </c>
       <c r="E602" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F602" t="inlineStr"/>
@@ -21438,7 +21438,7 @@
       </c>
       <c r="E604" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>a</t>
         </is>
       </c>
       <c r="F604" t="inlineStr">
@@ -21816,7 +21816,7 @@
       </c>
       <c r="E615" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>i</t>
         </is>
       </c>
       <c r="F615" t="inlineStr"/>
@@ -21884,7 +21884,7 @@
       </c>
       <c r="E617" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="F617" t="inlineStr"/>

</xml_diff>